<commit_message>
edited the excel document further, imported components for layout
</commit_message>
<xml_diff>
--- a/2nd_mainboard_bom/elektronik.xlsx
+++ b/2nd_mainboard_bom/elektronik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\Documents\GitHub\fiberprinter-electronics\2nd_mainboard_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3150D519-09B0-438F-B5D3-745FBE2F4FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AAD608-911E-4F99-B64B-35CB8F96C3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="BOM_DIFi2C_Printhead_20_07" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DifI2C!$A$1:$Q$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">DifI2C!$A$1:$Q$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="376">
   <si>
     <t>Alternative</t>
   </si>
@@ -226,9 +226,6 @@
     <t>https://www.amazon.de/-/en/Emitting-Electronic-Components-Assortment-Experience/dp/B0CSDDZJFQ/ref=sr_1_4?c=ts&amp;dib=eyJ2IjoiMSJ9.2GkvNPCeaKhaC6diij1KcbHfLOihmcR9MPolICWvOds4Pxgd68USwe8DqlWCYRX9E7T_Wzvyll1nv60h9UdFaVAe4LdMYk2HQcxQd7wSbd1O7GT2-3imf9uqJC7DsK6BinfscDVb6jZmxUjQiGr3xEtDbvmigDLWwlZIliOHLJ9U5_MicetPDftrr7oGvm14nZxfIyOC6mZc13j747MzLligfEK6PcS-Y57yiK3cvJN05qHUV40O2_Hw2JXWxQ6KIxZaFwXtvGu7hrLUyA7ziq0kgXimx818KQgtF-A0twU.KEk9ccj3Dwqiju9Y1TZPf-olJEs8Rv7uKLqS9ujZu2w&amp;dib_tag=se&amp;keywords=LED+Diodes&amp;qid=1721818074&amp;s=industrial&amp;sr=1-4&amp;ts_id=10388891031</t>
   </si>
   <si>
-    <t>Transistor</t>
-  </si>
-  <si>
     <t>Kapazitäten</t>
   </si>
   <si>
@@ -1094,6 +1091,84 @@
   </si>
   <si>
     <t xml:space="preserve">500mA, 2,9-17V, </t>
+  </si>
+  <si>
+    <t>Zener Diode</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/onsemi/SZ1SMB5927BT3G/9960092</t>
+  </si>
+  <si>
+    <t>SZ1SMB5927BT3G</t>
+  </si>
+  <si>
+    <t>12V, 3W</t>
+  </si>
+  <si>
+    <t>P-MOSFET als Verpolungsschutz</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/de/products/detail/vishay-siliconix/SQJ409EP-T1-GE3/7326286</t>
+  </si>
+  <si>
+    <t>SQJ409EP-T1_GE3</t>
+  </si>
+  <si>
+    <t>40V, max 60A Tc, max 68W Tc</t>
+  </si>
+  <si>
+    <t>Bestellbestand</t>
+  </si>
+  <si>
+    <t>N-MOSFET als Fan-Ansteuerung</t>
+  </si>
+  <si>
+    <t>https://www.digikey.de/en/products/detail/renesas-electronics-corporation/RJK0456DPB-00-J5/2694914</t>
+  </si>
+  <si>
+    <t>TP4</t>
+  </si>
+  <si>
+    <t>SMD Temperatursensor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/de/products/detail/abracon-llc/ABNTC-0805-103J-3950F-T/4245607</t>
+  </si>
+  <si>
+    <t>ABNTC-0805-103J-3950F-T</t>
+  </si>
+  <si>
+    <t>3950K, 200mW, -55 bis 125°C</t>
+  </si>
+  <si>
+    <t>40V, 50A Ta, Vgsmax +-20V</t>
+  </si>
+  <si>
+    <t>RJK0456DPB-00#J5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-40V zu 40V Buck </t>
+  </si>
+  <si>
+    <t>LM2679SX-12/NOPB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/en/products/detail/texas-instruments/LM2679SX-12-NOPB/366925</t>
+  </si>
+  <si>
+    <t>Ausgangsstrom 5A, 260kHz, 12V fixed</t>
+  </si>
+  <si>
+    <t>12V zu 5V Buck</t>
+  </si>
+  <si>
+    <t>https://www.digikey.at/en/products/detail/texas-instruments/LM22676MRX-5-0-NOPB/1951965</t>
+  </si>
+  <si>
+    <t>Ausgangsstrom 3A, 500kHz, 5V fixed</t>
+  </si>
+  <si>
+    <t>LM22676MRX-5.0/NOPB</t>
   </si>
 </sst>
 </file>
@@ -2448,8 +2523,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BC336CF2-AEC6-47D9-9EA5-9D5A14B19E97}" name="Table5" displayName="Table5" ref="A1:Q53" totalsRowShown="0" headerRowBorderDxfId="24" tableBorderDxfId="23">
-  <autoFilter ref="A1:Q53" xr:uid="{BC336CF2-AEC6-47D9-9EA5-9D5A14B19E97}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BC336CF2-AEC6-47D9-9EA5-9D5A14B19E97}" name="Table5" displayName="Table5" ref="A1:Q57" totalsRowShown="0" headerRowBorderDxfId="24" tableBorderDxfId="23">
+  <autoFilter ref="A1:Q57" xr:uid="{BC336CF2-AEC6-47D9-9EA5-9D5A14B19E97}"/>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{95952672-1FDA-4B59-A326-CD1AD2B01F86}" name="Alternative" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{8AD1858E-23FE-43D6-A875-8746EF5E6A17}" name="Bezeichnung" dataDxfId="21"/>
@@ -2772,11 +2847,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9C0DAD-F6B9-4E54-9647-FAF0BAA0CA58}">
-  <dimension ref="A1:Z69"/>
+  <dimension ref="A1:Z73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D36" sqref="D36"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2821,7 +2896,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H1" s="20" t="s">
         <v>6</v>
@@ -2857,20 +2932,20 @@
         <v>16</v>
       </c>
       <c r="T1" s="65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="U1" s="66"/>
       <c r="V1" s="36">
-        <f>SUMIFS(O9:O53,P9:P53, "Nicht Gekauft",Q9:Q53,"Benötigt")</f>
+        <f>SUMIFS(O9:O57,P9:P57, "Nicht Gekauft",Q9:Q57,"Benötigt")</f>
         <v>64.3</v>
       </c>
       <c r="X1" s="63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y1" s="64"/>
       <c r="Z1" s="26">
-        <f>SUM(O2:O53)</f>
-        <v>340.86000000000007</v>
+        <f>SUM(O2:O57)</f>
+        <v>358.83</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -2907,14 +2982,14 @@
         <v>1</v>
       </c>
       <c r="O2" s="45">
-        <f t="shared" ref="O2:O53" si="0">M2*N2</f>
+        <f t="shared" ref="O2:O57" si="0">M2*N2</f>
         <v>9.91</v>
       </c>
       <c r="P2" s="42" t="s">
         <v>24</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S2">
         <f>IF(AND(P2="Nicht Gekauft", Q2="Benötigt"), O2, 0)</f>
@@ -2923,7 +2998,7 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>26</v>
@@ -2966,12 +3041,12 @@
         <v>24</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
@@ -2980,10 +3055,10 @@
         <v>18</v>
       </c>
       <c r="D4" s="33" t="s">
+        <v>240</v>
+      </c>
+      <c r="E4" s="27" t="s">
         <v>241</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>242</v>
       </c>
       <c r="F4" s="2">
         <v>1.2</v>
@@ -2994,11 +3069,11 @@
       <c r="H4" s="2"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M4" s="3">
         <v>6.99</v>
@@ -3056,7 +3131,7 @@
         <v>24</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:S14" si="1">IF(AND(P5="Nicht Gekauft", Q5="Benötigt"), O5, 0)</f>
@@ -3065,19 +3140,19 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F6" s="2">
         <f>0.053*N6</f>
@@ -3093,7 +3168,7 @@
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M6" s="3">
         <v>8.5299999999999994</v>
@@ -3109,7 +3184,7 @@
         <v>24</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S6">
         <f t="shared" si="1"/>
@@ -3118,19 +3193,19 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="E7" s="27" t="s">
         <v>250</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>251</v>
       </c>
       <c r="F7" s="2">
         <v>0.17</v>
@@ -3145,7 +3220,7 @@
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M7" s="3">
         <v>6.73</v>
@@ -3160,24 +3235,24 @@
       <c r="P7" s="55"/>
       <c r="Q7" s="6"/>
       <c r="T7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F8" s="2">
         <v>0.35</v>
@@ -3192,7 +3267,7 @@
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="11" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M8" s="3">
         <v>7.4</v>
@@ -3207,24 +3282,24 @@
       <c r="P8" s="55"/>
       <c r="Q8" s="6"/>
       <c r="T8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>34</v>
@@ -3237,7 +3312,7 @@
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M9" s="3">
         <v>0.69</v>
@@ -3262,19 +3337,19 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>34</v>
@@ -3287,7 +3362,7 @@
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M10" s="3">
         <v>0.53</v>
@@ -3312,19 +3387,19 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>34</v>
@@ -3337,7 +3412,7 @@
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M11" s="3">
         <v>0.69</v>
@@ -3362,19 +3437,19 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>34</v>
@@ -3387,7 +3462,7 @@
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M12" s="3">
         <v>17.14</v>
@@ -3412,19 +3487,19 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="40" t="s">
         <v>34</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>34</v>
@@ -3437,7 +3512,7 @@
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M13" s="3">
         <v>8.0500000000000007</v>
@@ -3454,19 +3529,19 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>34</v>
@@ -3479,7 +3554,7 @@
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M14" s="3">
         <v>7.55</v>
@@ -3495,7 +3570,7 @@
         <v>24</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="R14" s="24"/>
       <c r="S14">
@@ -3505,19 +3580,19 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>34</v>
@@ -3530,7 +3605,7 @@
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M15" s="3">
         <v>0.22</v>
@@ -3548,19 +3623,19 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>34</v>
@@ -3573,7 +3648,7 @@
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="11" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="M16" s="3">
         <v>0.18</v>
@@ -3591,19 +3666,19 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>34</v>
@@ -3616,7 +3691,7 @@
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M17" s="3">
         <v>0.14000000000000001</v>
@@ -3635,16 +3710,16 @@
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C18" s="56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D18" s="40" t="s">
+        <v>340</v>
+      </c>
+      <c r="E18" s="27" t="s">
         <v>341</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>342</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>34</v>
@@ -3657,7 +3732,7 @@
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="M18" s="3">
         <v>0.84</v>
@@ -3675,19 +3750,19 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>34</v>
@@ -3699,10 +3774,10 @@
         <v>39</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L19" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M19" s="3">
         <v>3.24</v>
@@ -3720,19 +3795,19 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="40" t="s">
         <v>307</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>305</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>308</v>
-      </c>
       <c r="E20" s="27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>34</v>
@@ -3745,7 +3820,7 @@
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="M20" s="3">
         <v>1.7</v>
@@ -3763,19 +3838,19 @@
     </row>
     <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B21" s="27" t="s">
+        <v>310</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>299</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>312</v>
+      </c>
+      <c r="E21" s="27" t="s">
         <v>311</v>
-      </c>
-      <c r="C21" s="56" t="s">
-        <v>300</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>313</v>
-      </c>
-      <c r="E21" s="27" t="s">
-        <v>312</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>34</v>
@@ -3787,10 +3862,10 @@
         <v>39</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M21" s="3">
         <v>0.82</v>
@@ -3808,19 +3883,19 @@
     </row>
     <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C22" s="56" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D22" s="40" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>34</v>
@@ -3833,7 +3908,7 @@
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M22" s="3">
         <v>0.94</v>
@@ -3851,19 +3926,19 @@
     </row>
     <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="44" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C23" s="56" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D23" s="40" t="s">
+        <v>316</v>
+      </c>
+      <c r="E23" s="27" t="s">
         <v>317</v>
-      </c>
-      <c r="E23" s="27" t="s">
-        <v>318</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>34</v>
@@ -3876,7 +3951,7 @@
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M23" s="3">
         <v>1.33</v>
@@ -3895,16 +3970,16 @@
     <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="40" t="s">
         <v>328</v>
       </c>
-      <c r="C24" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>329</v>
-      </c>
       <c r="E24" s="27" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>34</v>
@@ -3917,7 +3992,7 @@
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M24" s="3">
         <v>2.04</v>
@@ -3934,16 +4009,16 @@
     </row>
     <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D25" s="40" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E25" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>34</v>
@@ -3955,10 +4030,10 @@
         <v>39</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="L25" s="11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M25" s="3">
         <v>0.1</v>
@@ -3974,19 +4049,19 @@
     </row>
     <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>34</v>
@@ -3998,10 +4073,10 @@
         <v>39</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="L26" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M26" s="3">
         <v>5.54</v>
@@ -4056,7 +4131,7 @@
         <v>57</v>
       </c>
       <c r="Q27" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S27">
         <f>IF(AND(P27="Nicht Gekauft", Q27="Benötigt"), O27, 0)</f>
@@ -4104,7 +4179,7 @@
         <v>57</v>
       </c>
       <c r="Q28" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S28">
         <f>IF(AND(P28="Nicht Gekauft", Q28="Benötigt"), O28, 0)</f>
@@ -4114,7 +4189,7 @@
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>53</v>
@@ -4123,7 +4198,7 @@
         <v>34</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>34</v>
@@ -4136,7 +4211,7 @@
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M29" s="3">
         <v>18.14</v>
@@ -4152,7 +4227,7 @@
         <v>57</v>
       </c>
       <c r="Q29" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S29">
         <f>IF(AND(P29="Nicht Gekauft", Q29="Benötigt"), O29, 0)</f>
@@ -4162,66 +4237,96 @@
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="27"/>
+        <v>359</v>
+      </c>
+      <c r="C30" s="56" t="s">
+        <v>358</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>367</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>366</v>
+      </c>
       <c r="F30" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+      <c r="J30" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="K30" s="4"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="13"/>
+      <c r="L30" s="11" t="s">
+        <v>360</v>
+      </c>
+      <c r="M30" s="3">
+        <v>2.91</v>
+      </c>
+      <c r="N30" s="13">
+        <v>2</v>
+      </c>
       <c r="O30" s="54">
-        <f>M30*N30</f>
-        <v>0</v>
+        <f t="shared" ref="O30:O38" si="4">M30*N30</f>
+        <v>5.82</v>
       </c>
       <c r="P30" s="55"/>
       <c r="Q30" s="6"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="27"/>
+      <c r="B31" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>330</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>356</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>357</v>
+      </c>
       <c r="F31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="J31" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="K31" s="4"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="13"/>
+      <c r="L31" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="M31" s="3">
+        <v>1.56</v>
+      </c>
+      <c r="N31" s="13">
+        <v>1</v>
+      </c>
       <c r="O31" s="54">
         <f>M31*N31</f>
-        <v>0</v>
+        <v>1.56</v>
       </c>
       <c r="P31" s="55"/>
       <c r="Q31" s="6"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44"/>
       <c r="B32" s="27" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="C32" s="56" t="s">
-        <v>331</v>
-      </c>
-      <c r="D32" s="40">
-        <v>824521241</v>
+        <v>330</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>352</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>334</v>
+        <v>353</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>34</v>
@@ -4230,21 +4335,21 @@
       <c r="H32" s="2"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4" t="s">
-        <v>335</v>
+        <v>39</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="11" t="s">
-        <v>332</v>
+        <v>351</v>
       </c>
       <c r="M32" s="3">
-        <v>0.3</v>
+        <v>0.47</v>
       </c>
       <c r="N32" s="13">
         <v>1</v>
       </c>
       <c r="O32" s="54">
-        <f>M32*N32</f>
-        <v>0.3</v>
+        <f t="shared" si="4"/>
+        <v>0.47</v>
       </c>
       <c r="P32" s="55"/>
       <c r="Q32" s="6"/>
@@ -4252,16 +4357,16 @@
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
       <c r="B33" s="27" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C33" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="40" t="s">
-        <v>337</v>
+        <v>330</v>
+      </c>
+      <c r="D33" s="40">
+        <v>824521241</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>34</v>
@@ -4270,21 +4375,21 @@
       <c r="H33" s="2"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4" t="s">
-        <v>39</v>
+        <v>334</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="11" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="M33" s="3">
-        <v>2.5499999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="N33" s="13">
         <v>1</v>
       </c>
       <c r="O33" s="54">
-        <f>M33*N33</f>
-        <v>2.5499999999999998</v>
+        <f t="shared" si="4"/>
+        <v>0.3</v>
       </c>
       <c r="P33" s="55"/>
       <c r="Q33" s="6"/>
@@ -4292,16 +4397,16 @@
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="27" t="s">
-        <v>343</v>
+        <v>368</v>
       </c>
       <c r="C34" s="56" t="s">
         <v>48</v>
       </c>
       <c r="D34" s="40" t="s">
-        <v>345</v>
+        <v>369</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>346</v>
+        <v>371</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>34</v>
@@ -4314,17 +4419,17 @@
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="11" t="s">
-        <v>344</v>
+        <v>370</v>
       </c>
       <c r="M34" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.79</v>
       </c>
       <c r="N34" s="13">
         <v>1</v>
       </c>
       <c r="O34" s="54">
         <f>M34*N34</f>
-        <v>4.5999999999999996</v>
+        <v>5.79</v>
       </c>
       <c r="P34" s="55"/>
       <c r="Q34" s="6"/>
@@ -4332,16 +4437,16 @@
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="27" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="C35" s="56" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="40" t="s">
-        <v>349</v>
+        <v>375</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>350</v>
+        <v>374</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -4352,336 +4457,303 @@
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="11" t="s">
-        <v>347</v>
+        <v>373</v>
       </c>
       <c r="M35" s="3">
-        <v>0.6</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="N35" s="13">
         <v>1</v>
       </c>
       <c r="O35" s="54">
         <f>M35*N35</f>
-        <v>0.6</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="P35" s="55"/>
       <c r="Q35" s="6"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
-      <c r="B36" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>38</v>
+      <c r="B36" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="C36" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>337</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8" t="s">
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="K36" s="8"/>
+      <c r="K36" s="4"/>
       <c r="L36" s="11" t="s">
+        <v>338</v>
+      </c>
+      <c r="M36" s="3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="N36" s="13">
+        <v>1</v>
+      </c>
+      <c r="O36" s="54">
+        <f t="shared" si="4"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="6"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="44"/>
+      <c r="B37" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>344</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K37" s="4"/>
+      <c r="L37" s="11" t="s">
+        <v>343</v>
+      </c>
+      <c r="M37" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N37" s="13">
+        <v>1</v>
+      </c>
+      <c r="O37" s="54">
+        <f t="shared" si="4"/>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P37" s="55"/>
+      <c r="Q37" s="6"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="44"/>
+      <c r="B38" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="C38" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>348</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>349</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K38" s="4"/>
+      <c r="L38" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="N38" s="13">
+        <v>1</v>
+      </c>
+      <c r="O38" s="54">
+        <f t="shared" si="4"/>
+        <v>0.6</v>
+      </c>
+      <c r="P38" s="55"/>
+      <c r="Q38" s="6"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A39" s="44"/>
+      <c r="B39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K39" s="8"/>
+      <c r="L39" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="M36" s="3">
+      <c r="M39" s="3">
         <v>0.88</v>
       </c>
-      <c r="N36" s="13">
+      <c r="N39" s="13">
         <v>10</v>
       </c>
-      <c r="O36" s="45">
+      <c r="O39" s="45">
         <f t="shared" si="0"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="P36" s="42" t="s">
+      <c r="P39" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="Q36" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="R36" s="22"/>
-      <c r="S36">
-        <f>IF(AND(P36="Nicht Gekauft", Q36="Benötigt"), O36, 0)</f>
+      <c r="Q39" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="R39" s="22"/>
+      <c r="S39">
+        <f t="shared" ref="S39:S44" si="5">IF(AND(P39="Nicht Gekauft", Q39="Benötigt"), O39, 0)</f>
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="44"/>
-      <c r="B37" s="2" t="s">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A40" s="44"/>
+      <c r="B40" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8" t="s">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K37" s="8"/>
-      <c r="L37" s="11" t="s">
+      <c r="K40" s="8"/>
+      <c r="L40" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M40" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="N37" s="13">
+      <c r="N40" s="13">
         <v>4</v>
       </c>
-      <c r="O37" s="45">
+      <c r="O40" s="45">
         <f t="shared" si="0"/>
         <v>2.2799999999999998</v>
       </c>
-      <c r="P37" s="42" t="s">
+      <c r="P40" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="Q37" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="R37" s="22"/>
-      <c r="S37">
-        <f>IF(AND(P37="Nicht Gekauft", Q37="Benötigt"), O37, 0)</f>
+      <c r="Q40" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="R40" s="22"/>
+      <c r="S40">
+        <f t="shared" si="5"/>
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="44"/>
-      <c r="B38" s="2" t="s">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A41" s="44"/>
+      <c r="B41" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8" t="s">
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="K38" s="8"/>
-      <c r="L38" s="11" t="s">
+      <c r="K41" s="8"/>
+      <c r="L41" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="M38" s="3">
+      <c r="M41" s="3">
         <v>0.55000000000000004</v>
       </c>
-      <c r="N38" s="13">
+      <c r="N41" s="13">
         <v>4</v>
       </c>
-      <c r="O38" s="45">
+      <c r="O41" s="45">
         <f t="shared" si="0"/>
         <v>2.2000000000000002</v>
       </c>
-      <c r="P38" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q38" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="R38" s="22"/>
-      <c r="S38">
-        <f>IF(AND(P38="Nicht Gekauft", Q38="Benötigt"), O38, 0)</f>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K39" s="4"/>
-      <c r="L39" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="M39" s="3">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="N39" s="13">
-        <v>2</v>
-      </c>
-      <c r="O39" s="45">
-        <f t="shared" si="0"/>
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="P39" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q39" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R39" s="22"/>
-      <c r="S39">
-        <f>IF(AND(P39="Nicht Gekauft", Q39="Benötigt"), O39, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F40" s="2">
-        <v>4.0000000000000002E-4</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="4"/>
-      <c r="J40" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K40" s="4"/>
-      <c r="L40" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="M40" s="3">
-        <v>4.49</v>
-      </c>
-      <c r="N40" s="13">
-        <v>2</v>
-      </c>
-      <c r="O40" s="45">
-        <f t="shared" si="0"/>
-        <v>8.98</v>
-      </c>
-      <c r="P40" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q40" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R40" s="22"/>
-      <c r="S40">
-        <f>IF(AND(P40="Nicht Gekauft", Q40="Benötigt"), O40, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="44" t="s">
-        <v>91</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K41" s="4"/>
-      <c r="L41" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="M41" s="3">
-        <v>2.81</v>
-      </c>
-      <c r="N41" s="13">
-        <v>4</v>
-      </c>
-      <c r="O41" s="45">
-        <f t="shared" si="0"/>
-        <v>11.24</v>
-      </c>
       <c r="P41" s="42" t="s">
         <v>24</v>
       </c>
       <c r="Q41" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="R41" s="22"/>
       <c r="S41">
-        <f>IF(AND(P41="Nicht Gekauft", Q41="Benötigt"), O41, 0)</f>
-        <v>11.24</v>
+        <f t="shared" si="5"/>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="E42" s="27" t="s">
-        <v>256</v>
+      <c r="E42" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>34</v>
@@ -4690,82 +4762,100 @@
       <c r="H42" s="2"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4" t="s">
-        <v>243</v>
+        <v>39</v>
       </c>
       <c r="K42" s="4"/>
       <c r="L42" s="11" t="s">
-        <v>254</v>
+        <v>84</v>
       </c>
       <c r="M42" s="3">
-        <v>5.99</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="N42" s="13">
-        <v>4</v>
-      </c>
-      <c r="O42" s="54">
-        <f>M42*N42</f>
-        <v>23.96</v>
-      </c>
-      <c r="P42" s="55"/>
-      <c r="Q42" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="O42" s="45">
+        <f t="shared" si="0"/>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="P42" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q42" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="R42" s="22"/>
+      <c r="S42">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="2" t="s">
-        <v>34</v>
+      <c r="E43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="2">
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4" t="s">
-        <v>243</v>
+        <v>39</v>
       </c>
       <c r="K43" s="4"/>
       <c r="L43" s="11" t="s">
-        <v>265</v>
+        <v>89</v>
       </c>
       <c r="M43" s="3">
-        <v>2.99</v>
+        <v>4.49</v>
       </c>
       <c r="N43" s="13">
-        <v>4</v>
-      </c>
-      <c r="O43" s="54">
-        <f>M43*N43</f>
-        <v>11.96</v>
-      </c>
-      <c r="P43" s="55"/>
-      <c r="Q43" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="O43" s="45">
+        <f t="shared" si="0"/>
+        <v>8.98</v>
+      </c>
+      <c r="P43" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="R43" s="22"/>
+      <c r="S43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="C44" s="56" t="s">
-        <v>82</v>
-      </c>
-      <c r="D44" s="40" t="s">
-        <v>258</v>
-      </c>
-      <c r="E44" t="s">
-        <v>263</v>
+        <v>90</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>34</v>
@@ -4774,41 +4864,49 @@
       <c r="H44" s="2"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="K44" s="4"/>
       <c r="L44" s="11" t="s">
-        <v>257</v>
+        <v>93</v>
       </c>
       <c r="M44" s="3">
-        <v>0.1</v>
+        <v>2.81</v>
       </c>
       <c r="N44" s="13">
-        <v>10</v>
-      </c>
-      <c r="O44" s="54">
-        <f>M44*N44</f>
-        <v>1</v>
-      </c>
-      <c r="P44" s="55"/>
-      <c r="Q44" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="O44" s="45">
+        <f t="shared" si="0"/>
+        <v>11.24</v>
+      </c>
+      <c r="P44" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q44" s="6" t="s">
+        <v>231</v>
+      </c>
       <c r="R44" s="22"/>
+      <c r="S44">
+        <f t="shared" si="5"/>
+        <v>11.24</v>
+      </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="C45" s="56" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="D45" s="40" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="E45" s="27" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>34</v>
@@ -4817,21 +4915,21 @@
       <c r="H45" s="2"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4" t="s">
-        <v>39</v>
+        <v>242</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="11" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="M45" s="3">
-        <v>5.54</v>
+        <v>5.99</v>
       </c>
       <c r="N45" s="13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O45" s="54">
         <f>M45*N45</f>
-        <v>5.54</v>
+        <v>23.96</v>
       </c>
       <c r="P45" s="55"/>
       <c r="Q45" s="6"/>
@@ -4839,20 +4937,18 @@
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>267</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="39" t="s">
-        <v>115</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>116</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D46" s="40" t="s">
+        <v>265</v>
+      </c>
+      <c r="E46" s="27"/>
       <c r="F46" s="2" t="s">
         <v>34</v>
       </c>
@@ -4860,48 +4956,41 @@
       <c r="H46" s="2"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4" t="s">
-        <v>39</v>
+        <v>242</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="11" t="s">
-        <v>117</v>
+        <v>264</v>
       </c>
       <c r="M46" s="3">
-        <v>16.100000000000001</v>
+        <v>2.99</v>
       </c>
       <c r="N46" s="13">
-        <v>1</v>
-      </c>
-      <c r="O46" s="45">
-        <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
-      </c>
-      <c r="P46" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q46" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="S46">
-        <f>IF(AND(P46="Nicht Gekauft", Q46="Benötigt"), O46, 0)</f>
-        <v>16.100000000000001</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="O46" s="54">
+        <f>M46*N46</f>
+        <v>11.96</v>
+      </c>
+      <c r="P46" s="55"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="22"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>272</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="33" t="s">
-        <v>271</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>116</v>
+        <v>79</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D47" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="E47" t="s">
+        <v>262</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>34</v>
@@ -4910,40 +4999,41 @@
       <c r="H47" s="2"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4" t="s">
-        <v>269</v>
+        <v>39</v>
       </c>
       <c r="K47" s="4"/>
       <c r="L47" s="11" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="M47" s="3">
-        <v>6.99</v>
+        <v>0.1</v>
       </c>
       <c r="N47" s="13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="O47" s="54">
         <f>M47*N47</f>
-        <v>6.99</v>
+        <v>1</v>
       </c>
       <c r="P47" s="55"/>
       <c r="Q47" s="6"/>
+      <c r="R47" s="22"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
-        <v>268</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="33" t="s">
-        <v>273</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>274</v>
+        <v>79</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D48" s="40" t="s">
+        <v>259</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>263</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>34</v>
@@ -4952,44 +5042,43 @@
       <c r="H48" s="2"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4" t="s">
-        <v>275</v>
+        <v>39</v>
       </c>
       <c r="K48" s="4"/>
       <c r="L48" s="11" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="M48" s="3">
-        <v>9.33</v>
+        <v>5.54</v>
       </c>
       <c r="N48" s="13">
         <v>1</v>
       </c>
       <c r="O48" s="54">
         <f>M48*N48</f>
-        <v>9.33</v>
+        <v>5.54</v>
       </c>
       <c r="P48" s="55"/>
       <c r="Q48" s="6"/>
+      <c r="R48" s="22"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="33" t="s">
-        <v>278</v>
+        <v>361</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="C49" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D49" s="40" t="s">
+        <v>364</v>
       </c>
       <c r="E49" s="27" t="s">
-        <v>279</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="F49" s="2"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="4"/>
@@ -4998,36 +5087,37 @@
       </c>
       <c r="K49" s="4"/>
       <c r="L49" s="11" t="s">
-        <v>280</v>
+        <v>363</v>
       </c>
       <c r="M49" s="3">
-        <v>3.39</v>
+        <v>0.19</v>
       </c>
       <c r="N49" s="13">
         <v>1</v>
       </c>
       <c r="O49" s="54">
         <f>M49*N49</f>
-        <v>3.39</v>
+        <v>0.19</v>
       </c>
       <c r="P49" s="55"/>
       <c r="Q49" s="6"/>
+      <c r="R49" s="22"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D50" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" s="27" t="s">
-        <v>69</v>
+        <v>266</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>34</v>
@@ -5036,48 +5126,48 @@
       <c r="H50" s="2"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="K50" s="4"/>
       <c r="L50" s="11" t="s">
-        <v>70</v>
+        <v>116</v>
       </c>
       <c r="M50" s="3">
-        <v>16.13</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="N50" s="13">
         <v>1</v>
       </c>
       <c r="O50" s="45">
         <f t="shared" si="0"/>
-        <v>16.13</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="P50" s="42" t="s">
         <v>24</v>
       </c>
       <c r="Q50" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="S50">
         <f>IF(AND(P50="Nicht Gekauft", Q50="Benötigt"), O50, 0)</f>
-        <v>16.13</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B51" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="E51" s="27" t="s">
-        <v>74</v>
+        <v>271</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>270</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>34</v>
@@ -5086,44 +5176,40 @@
       <c r="H51" s="2"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4" t="s">
-        <v>39</v>
+        <v>268</v>
       </c>
       <c r="K51" s="4"/>
       <c r="L51" s="11" t="s">
-        <v>75</v>
+        <v>269</v>
       </c>
       <c r="M51" s="3">
-        <v>2.97</v>
+        <v>6.99</v>
       </c>
       <c r="N51" s="13">
-        <v>2</v>
-      </c>
-      <c r="O51" s="45">
-        <f t="shared" si="0"/>
-        <v>5.94</v>
-      </c>
-      <c r="P51" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q51" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="O51" s="54">
+        <f>M51*N51</f>
+        <v>6.99</v>
+      </c>
+      <c r="P51" s="55"/>
+      <c r="Q51" s="6"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="44" t="s">
-        <v>71</v>
-      </c>
-      <c r="B52" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C52" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D52" s="40" t="s">
-        <v>76</v>
-      </c>
-      <c r="E52" s="27" t="s">
-        <v>74</v>
+        <v>267</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="33" t="s">
+        <v>272</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>273</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>34</v>
@@ -5132,145 +5218,312 @@
       <c r="H52" s="2"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4" t="s">
-        <v>39</v>
+        <v>274</v>
       </c>
       <c r="K52" s="4"/>
       <c r="L52" s="11" t="s">
-        <v>77</v>
+        <v>275</v>
       </c>
       <c r="M52" s="3">
+        <v>9.33</v>
+      </c>
+      <c r="N52" s="13">
+        <v>1</v>
+      </c>
+      <c r="O52" s="54">
+        <f>M52*N52</f>
+        <v>9.33</v>
+      </c>
+      <c r="P52" s="55"/>
+      <c r="Q52" s="6"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>278</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K53" s="4"/>
+      <c r="L53" s="11" t="s">
+        <v>279</v>
+      </c>
+      <c r="M53" s="3">
+        <v>3.39</v>
+      </c>
+      <c r="N53" s="13">
+        <v>1</v>
+      </c>
+      <c r="O53" s="54">
+        <f>M53*N53</f>
+        <v>3.39</v>
+      </c>
+      <c r="P53" s="55"/>
+      <c r="Q53" s="6"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D54" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54" s="4"/>
+      <c r="L54" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M54" s="3">
+        <v>16.13</v>
+      </c>
+      <c r="N54" s="13">
+        <v>1</v>
+      </c>
+      <c r="O54" s="45">
+        <f t="shared" si="0"/>
+        <v>16.13</v>
+      </c>
+      <c r="P54" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q54" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="S54">
+        <f>IF(AND(P54="Nicht Gekauft", Q54="Benötigt"), O54, 0)</f>
+        <v>16.13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D55" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K55" s="4"/>
+      <c r="L55" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="M55" s="3">
+        <v>2.97</v>
+      </c>
+      <c r="N55" s="13">
+        <v>2</v>
+      </c>
+      <c r="O55" s="45">
+        <f t="shared" si="0"/>
+        <v>5.94</v>
+      </c>
+      <c r="P55" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q55" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A56" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K56" s="4"/>
+      <c r="L56" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="M56" s="3">
         <v>5.92</v>
       </c>
-      <c r="N52" s="13">
-        <v>1</v>
-      </c>
-      <c r="O52" s="45">
+      <c r="N56" s="13">
+        <v>1</v>
+      </c>
+      <c r="O56" s="45">
         <f t="shared" si="0"/>
         <v>5.92</v>
       </c>
-      <c r="P52" s="42" t="s">
+      <c r="P56" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="Q52" s="6" t="s">
+      <c r="Q56" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="46" t="s">
+    <row r="57" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="B53" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="C53" s="47" t="s">
-        <v>65</v>
-      </c>
-      <c r="D53" s="48" t="s">
+      <c r="C57" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D57" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E57" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="F57" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="47"/>
+      <c r="H57" s="47"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="K57" s="49"/>
+      <c r="L57" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="E53" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="F53" s="47" t="s">
-        <v>34</v>
-      </c>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
-      <c r="I53" s="49"/>
-      <c r="J53" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="K53" s="49"/>
-      <c r="L53" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="M53" s="51">
+      <c r="M57" s="51">
         <v>2.64</v>
       </c>
-      <c r="N53" s="52">
-        <v>1</v>
-      </c>
-      <c r="O53" s="53">
+      <c r="N57" s="52">
+        <v>1</v>
+      </c>
+      <c r="O57" s="53">
         <f t="shared" si="0"/>
         <v>2.64</v>
       </c>
-      <c r="P53" s="42" t="s">
+      <c r="P57" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="Q53" s="6" t="s">
+      <c r="Q57" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="S53">
-        <f>IF(AND(P53="Nicht Gekauft", Q53="Benötigt"), O53, 0)</f>
+      <c r="S57">
+        <f>IF(AND(P57="Nicht Gekauft", Q57="Benötigt"), O57, 0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" s="58"/>
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="59"/>
-      <c r="J54" s="59"/>
-      <c r="K54" s="59"/>
-      <c r="L54" s="60"/>
-      <c r="M54" s="61"/>
-      <c r="N54" s="62"/>
-      <c r="O54" s="61"/>
-      <c r="P54" s="62"/>
-    </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="56" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E56" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="F56" s="21">
-        <f>SUBTOTAL(9,F1:F53)</f>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A58" s="58"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
+      <c r="E58" s="58"/>
+      <c r="F58" s="58"/>
+      <c r="G58" s="58"/>
+      <c r="H58" s="58"/>
+      <c r="I58" s="59"/>
+      <c r="J58" s="59"/>
+      <c r="K58" s="59"/>
+      <c r="L58" s="60"/>
+      <c r="M58" s="61"/>
+      <c r="N58" s="62"/>
+      <c r="O58" s="61"/>
+      <c r="P58" s="62"/>
+    </row>
+    <row r="59" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E60" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="F60" s="21">
+        <f>SUBTOTAL(9,F1:F57)</f>
         <v>3.3824000000000001</v>
       </c>
-      <c r="G56" s="57"/>
-      <c r="M56" s="69" t="s">
-        <v>234</v>
-      </c>
-      <c r="N56" s="70"/>
-      <c r="O56" s="38">
-        <f>SUBTOTAL(9,O1:O53)</f>
-        <v>340.86000000000007</v>
-      </c>
-    </row>
-    <row r="58" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H58" s="7"/>
-    </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H59" s="7"/>
-      <c r="M59" s="67" t="s">
+      <c r="G60" s="57"/>
+      <c r="M60" s="69" t="s">
         <v>233</v>
       </c>
-      <c r="N59" s="68"/>
-      <c r="O59" s="25">
-        <f>SUBTOTAL(9,S1:S53)</f>
-        <v>115.32</v>
-      </c>
-    </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N60" s="70"/>
+      <c r="O60" s="38">
+        <f>SUBTOTAL(9,O1:O57)</f>
+        <v>358.83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H62" s="7"/>
     </row>
     <row r="63" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H64" s="7"/>
+      <c r="M63" s="67" t="s">
+        <v>232</v>
+      </c>
+      <c r="N63" s="68"/>
+      <c r="O63" s="25">
+        <f>SUBTOTAL(9,S1:S57)</f>
+        <v>115.32</v>
+      </c>
     </row>
     <row r="65" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H65" s="7"/>
-      <c r="L65" s="23"/>
     </row>
     <row r="66" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H66" s="7"/>
@@ -5283,18 +5536,31 @@
     </row>
     <row r="69" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H69" s="7"/>
-      <c r="I69" s="7" t="s">
-        <v>122</v>
+      <c r="L69" s="23"/>
+    </row>
+    <row r="70" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="8:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H73" s="7"/>
+      <c r="I73" s="7" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="X1:Y1"/>
     <mergeCell ref="T1:U1"/>
-    <mergeCell ref="M59:N59"/>
-    <mergeCell ref="M56:N56"/>
+    <mergeCell ref="M63:N63"/>
+    <mergeCell ref="M60:N60"/>
   </mergeCells>
-  <conditionalFormatting sqref="P61:P1048576 P1:P24 P27:P59">
+  <conditionalFormatting sqref="P1:P24 P27:P63 P65:P1048576">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Nicht Gekauft"</formula>
     </cfRule>
@@ -5310,7 +5576,7 @@
       <formula>"Gekauft"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q24 Q27:Q54">
+  <conditionalFormatting sqref="Q2:Q24 Q27:Q58">
     <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Nicht benötigt"</formula>
     </cfRule>
@@ -5319,27 +5585,27 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24 Q27:Q54" xr:uid="{DF639F38-DCBF-4FB0-9016-BE70B5447265}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q24 Q27:Q58" xr:uid="{DF639F38-DCBF-4FB0-9016-BE70B5447265}">
       <formula1>"Benötigt,Nicht benötigt"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24 P27:P54" xr:uid="{BB82D80E-695D-4A38-A148-48463DFE8321}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P24 P27:P58" xr:uid="{BB82D80E-695D-4A38-A148-48463DFE8321}">
       <formula1>"Gekauft,Nicht Gekauft"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{134576B2-6870-47F8-80B5-95CA9B97F9E2}"/>
-    <hyperlink ref="L36" r:id="rId2" xr:uid="{F3AD9EFC-A933-40C0-B3D6-105AE81F974F}"/>
-    <hyperlink ref="L37" r:id="rId3" xr:uid="{0B081703-43B3-49C1-ABA0-60C83F319C14}"/>
-    <hyperlink ref="L38" r:id="rId4" xr:uid="{A386B0E7-0270-440F-94E8-1A585C273E01}"/>
+    <hyperlink ref="L39" r:id="rId2" xr:uid="{F3AD9EFC-A933-40C0-B3D6-105AE81F974F}"/>
+    <hyperlink ref="L40" r:id="rId3" xr:uid="{0B081703-43B3-49C1-ABA0-60C83F319C14}"/>
+    <hyperlink ref="L41" r:id="rId4" xr:uid="{A386B0E7-0270-440F-94E8-1A585C273E01}"/>
     <hyperlink ref="L27" r:id="rId5" xr:uid="{6E8ED221-C460-4F2D-A839-674D0DD8E486}"/>
     <hyperlink ref="L28" r:id="rId6" display="https://www.amazon.de/-/en/Emitting-Electronic-Components-Assortment-Experience/dp/B0CSDDZJFQ/ref=sr_1_4?c=ts&amp;dib=eyJ2IjoiMSJ9.2GkvNPCeaKhaC6diij1KcbHfLOihmcR9MPolICWvOds4Pxgd68USwe8DqlWCYRX9E7T_Wzvyll1nv60h9UdFaVAe4LdMYk2HQcxQd7wSbd1O7GT2-3imf9uqJC7DsK6BinfscDVb6jZmxUjQiGr3xEtDbvmigDLWwlZIliOHLJ9U5_MicetPDftrr7oGvm14nZxfIyOC6mZc13j747MzLligfEK6PcS-Y57yiK3cvJN05qHUV40O2_Hw2JXWxQ6KIxZaFwXtvGu7hrLUyA7ziq0kgXimx818KQgtF-A0twU.KEk9ccj3Dwqiju9Y1TZPf-olJEs8Rv7uKLqS9ujZu2w&amp;dib_tag=se&amp;keywords=LED+Diodes&amp;qid=1721818074&amp;s=industrial&amp;sr=1-4&amp;ts_id=10388891031" xr:uid="{DF5ECAD5-98DD-434D-AC21-981A114328F6}"/>
-    <hyperlink ref="L50" r:id="rId7" display="https://www.amazon.de/-/en/KeeYees-Adapter-Prototype-TQFP100-QQQN444/dp/B085LC6ZSY/ref=sr_1_17?crid=1T3EHGG52EF9V&amp;dib=eyJ2IjoiMSJ9.nRnqv21X2z_-T0RW4ed0Tax59DHuIK9be7jBvZ221ZgEzBBfXYLvZQgCHkBNi1SpzCv3sBmo5QK4GzT_rqJOXpksQlaGFLKbUAwj70xEI2jQcZyuEh3Pdl88nTe7A7OAQBztbOjeTzHxuxaSoFmE0O1nXdR67iZOW8EEA3ZhgqxrQ2srlihg5rC7H1JC_UCMWv1IXNZEh7N9K4Mt2NallWFPXa8XlZ5gMROKCd_32IPKp70Hx8ybO_vAHfCb6hNezayFfGQ3wMbsHix17cojW93IyixK8YMRj5z0JMiT3_M.5eq3Z6976gWt1o83vhxwbBR-r-mwWYKu_zQecQ3Zvf8&amp;dib_tag=se&amp;keywords=smd+tht&amp;qid=1721976524&amp;sprefix=smd+tht+test%2Caps%2C86&amp;sr=8-17" xr:uid="{3D8950E4-A562-41A1-A7F1-9202B2ABF32B}"/>
-    <hyperlink ref="L51" r:id="rId8" xr:uid="{9A0B0992-EB9B-485C-8743-AB5373B961C2}"/>
-    <hyperlink ref="L52" r:id="rId9" display="https://octopart.com/opatz8j6/a1?t=m3MKmMPlltUlOaMyNv3oKjBZdMKsW17dy_Ut3gz9BnX84ucyH8jy82DqArAu4BfwE0Hye-7iCLl8KH0frtEOW989MvS5s7ux5kMEtqEpjHhVRKNi28LZWUZICT7zsPBmwWgjTMYjcOOVdfJXu9Y10LLBHTNi5TEX6yjYVdKqsLNYSCadhn_Li_cFolA9fQUsggKr6BxWSw52ZDMMaokL6vRljCt85LJQd_a1rKyujcjn71swSSETRfaBoDVV_VXxkQ" xr:uid="{CB92E7DB-FA84-47D1-9C2D-C21CBE2C47E3}"/>
-    <hyperlink ref="L53" r:id="rId10" xr:uid="{B67FB571-1B87-4184-A2B3-AF411BD87D35}"/>
-    <hyperlink ref="L40" r:id="rId11" xr:uid="{57963C92-CE56-4D91-B1F1-7FA05F5BC3A8}"/>
-    <hyperlink ref="L39" r:id="rId12" xr:uid="{9D795571-0999-43FF-9A1F-496FF99C86C0}"/>
-    <hyperlink ref="L41" r:id="rId13" xr:uid="{8465788D-FDE3-460C-960F-435D2FB5F396}"/>
+    <hyperlink ref="L54" r:id="rId7" display="https://www.amazon.de/-/en/KeeYees-Adapter-Prototype-TQFP100-QQQN444/dp/B085LC6ZSY/ref=sr_1_17?crid=1T3EHGG52EF9V&amp;dib=eyJ2IjoiMSJ9.nRnqv21X2z_-T0RW4ed0Tax59DHuIK9be7jBvZ221ZgEzBBfXYLvZQgCHkBNi1SpzCv3sBmo5QK4GzT_rqJOXpksQlaGFLKbUAwj70xEI2jQcZyuEh3Pdl88nTe7A7OAQBztbOjeTzHxuxaSoFmE0O1nXdR67iZOW8EEA3ZhgqxrQ2srlihg5rC7H1JC_UCMWv1IXNZEh7N9K4Mt2NallWFPXa8XlZ5gMROKCd_32IPKp70Hx8ybO_vAHfCb6hNezayFfGQ3wMbsHix17cojW93IyixK8YMRj5z0JMiT3_M.5eq3Z6976gWt1o83vhxwbBR-r-mwWYKu_zQecQ3Zvf8&amp;dib_tag=se&amp;keywords=smd+tht&amp;qid=1721976524&amp;sprefix=smd+tht+test%2Caps%2C86&amp;sr=8-17" xr:uid="{3D8950E4-A562-41A1-A7F1-9202B2ABF32B}"/>
+    <hyperlink ref="L55" r:id="rId8" xr:uid="{9A0B0992-EB9B-485C-8743-AB5373B961C2}"/>
+    <hyperlink ref="L56" r:id="rId9" display="https://octopart.com/opatz8j6/a1?t=m3MKmMPlltUlOaMyNv3oKjBZdMKsW17dy_Ut3gz9BnX84ucyH8jy82DqArAu4BfwE0Hye-7iCLl8KH0frtEOW989MvS5s7ux5kMEtqEpjHhVRKNi28LZWUZICT7zsPBmwWgjTMYjcOOVdfJXu9Y10LLBHTNi5TEX6yjYVdKqsLNYSCadhn_Li_cFolA9fQUsggKr6BxWSw52ZDMMaokL6vRljCt85LJQd_a1rKyujcjn71swSSETRfaBoDVV_VXxkQ" xr:uid="{CB92E7DB-FA84-47D1-9C2D-C21CBE2C47E3}"/>
+    <hyperlink ref="L57" r:id="rId10" xr:uid="{B67FB571-1B87-4184-A2B3-AF411BD87D35}"/>
+    <hyperlink ref="L43" r:id="rId11" xr:uid="{57963C92-CE56-4D91-B1F1-7FA05F5BC3A8}"/>
+    <hyperlink ref="L42" r:id="rId12" xr:uid="{9D795571-0999-43FF-9A1F-496FF99C86C0}"/>
+    <hyperlink ref="L44" r:id="rId13" xr:uid="{8465788D-FDE3-460C-960F-435D2FB5F396}"/>
     <hyperlink ref="L9" r:id="rId14" xr:uid="{A9D6150D-3C06-4D81-AD60-047F4F409296}"/>
     <hyperlink ref="L10" r:id="rId15" xr:uid="{411A7094-1AC1-4084-ABE4-5C0060EC1A2D}"/>
     <hyperlink ref="L11" r:id="rId16" xr:uid="{3DDB6C5A-7DB3-4C65-B604-D02293535F49}"/>
@@ -5347,11 +5613,11 @@
     <hyperlink ref="L14" r:id="rId18" display="https://www.amazon.de/Sourcingmap%C2%AE-rechten-Einreihige-Stiftleiste-PCB-Steckverbinder-Black-Silver-Tone/dp/B01MZE0XGZ/ref=sr_1_2?__mk_de_DE=%C3%85M%C3%85%C5%BD%C3%95%C3%91&amp;crid=30UQ32XMVEOXN&amp;dib=eyJ2IjoiMSJ9.yl2DLiqdSMCvFJDFZqTKgUH67xEpPOL40VD2AFIkG-UVuzOI9AaqWj6c1QgSiCn7hk05FWychE9FePelrXDhrx8em4i4SmadkDqm8tD_rw9vdmMLNh68adnrUu-GEIXx3JcPfOHWruMciXYFg7IYLW6ouYqX2t7OpXQyrIWp9qfW6VVlyLcSOlxu99s5ni58gvswEZke7glukuR6cKzmRpHdyVh-uVExobnZmGNZHApgLz7h-ZMXrQq6hEE3srvrZrSBQQDvA_NN-Yhpyev3ZGXq76pUZSA4LFbhGazIe6s.zFPbYnk3PEWXUlrobf2fvrzvsV48VUdck_WWv7Vof8w&amp;dib_tag=se&amp;keywords=pin+header+winkel&amp;qid=1721383256&amp;sprefix=pinheader+winkel%2Caps%2C104&amp;sr=8-2" xr:uid="{2B77B7B0-D725-4006-ADC9-9301FF6B0095}"/>
     <hyperlink ref="L6" r:id="rId19" xr:uid="{56E44BCE-942A-4E32-8574-907151789664}"/>
     <hyperlink ref="L29" r:id="rId20" display="https://www.amazon.de/-/en/Capacitor-Assortment-Electrolytic-Capacitors-Aluminium/dp/B09QH1RLRS/ref=sr_1_5?crid=MXP52929GLQF&amp;dib=eyJ2IjoiMSJ9.RVY4AKzuAKEuJTtsjJJyAjJN9dTUKTzMyAFbwbFQ9TN9T9C6FQ6jEbz5YhVbDbdMkSnm5DKnBIJl_XR3nCkiZvZ8qBxyFkP5DE-H0QH2e0LU-xb6fKOU3K5dgabojwYdkqXPT8_Crzfg3wCzX6NZ0kNe4l1kiD1OOIvn4RVD6J_mrfygtByox4gT8deaDI5vmVCNWQjuvIbrESS2VQBYV3j5LwPPKCdDp_ieM0jSKHfCHtdVZxtyW1QcrFUTBltGEo3DHrbbHGndykkj50wTc98L8p5Hi8W9aHQR3MNFSAM.C6EdXg8VemgyEusoxnNl57g3RPDCQROGEsYtZcxEtls&amp;dib_tag=se&amp;keywords=Kondensator&amp;qid=1722243539&amp;sprefix=kondensator%2Caps%2C95&amp;sr=8-5&amp;th=1" xr:uid="{0F5D6938-DDE4-45D4-8279-23754047E314}"/>
-    <hyperlink ref="L46" r:id="rId21" xr:uid="{D632E27D-8B4B-473B-9951-117DBC2C36E0}"/>
+    <hyperlink ref="L50" r:id="rId21" xr:uid="{D632E27D-8B4B-473B-9951-117DBC2C36E0}"/>
     <hyperlink ref="L3" r:id="rId22" xr:uid="{C49F6822-A4DD-42C2-B3BF-0381D137937C}"/>
     <hyperlink ref="L5" r:id="rId23" xr:uid="{BF0FEABB-4850-4BC5-A11D-D889C6B926FD}"/>
     <hyperlink ref="L7" r:id="rId24" xr:uid="{21389653-C0FE-46E1-B136-04B9A0DE28C5}"/>
-    <hyperlink ref="L42" r:id="rId25" xr:uid="{1242A3DC-9FDC-4C47-9270-1B4A92E75E73}"/>
+    <hyperlink ref="L45" r:id="rId25" xr:uid="{1242A3DC-9FDC-4C47-9270-1B4A92E75E73}"/>
     <hyperlink ref="L25" r:id="rId26" xr:uid="{3ED73B15-E49B-4E21-BF8D-06828BFBADB2}"/>
     <hyperlink ref="L8" r:id="rId27" xr:uid="{E62708AD-A075-4D9D-9BC8-2CBD617B66EE}"/>
     <hyperlink ref="L26" r:id="rId28" xr:uid="{488C7B18-56E0-4061-83E3-FAA678922DF9}"/>
@@ -5382,36 +5648,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="C1" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="D1" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="E1" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="F1" s="28" t="s">
         <v>127</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="C2" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="D2" s="28" t="s">
         <v>131</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>132</v>
       </c>
       <c r="E2" s="28">
         <v>1</v>
@@ -5420,16 +5686,16 @@
     </row>
     <row r="3" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="C3" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="D3" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>136</v>
       </c>
       <c r="E3" s="28">
         <v>1</v>
@@ -5437,13 +5703,13 @@
     </row>
     <row r="4" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="28" t="s">
-        <v>138</v>
-      </c>
       <c r="C4" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>34</v>
@@ -5454,16 +5720,16 @@
     </row>
     <row r="5" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="C5" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="D5" s="28" t="s">
         <v>141</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>142</v>
       </c>
       <c r="E5" s="28">
         <v>1</v>
@@ -5472,16 +5738,16 @@
     </row>
     <row r="6" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="C6" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>144</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>145</v>
       </c>
       <c r="E6" s="28">
         <v>1</v>
@@ -5489,16 +5755,16 @@
     </row>
     <row r="7" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="C7" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="28" t="s">
         <v>147</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="D7" s="28" t="s">
-        <v>148</v>
       </c>
       <c r="E7" s="28">
         <v>1</v>
@@ -5506,16 +5772,16 @@
     </row>
     <row r="8" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="B8" s="28" t="s">
-        <v>150</v>
-      </c>
       <c r="C8" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="28">
         <v>1</v>
@@ -5523,16 +5789,16 @@
     </row>
     <row r="9" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>152</v>
-      </c>
       <c r="C9" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E9" s="28">
         <v>1</v>
@@ -5540,16 +5806,16 @@
     </row>
     <row r="10" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="28" t="s">
-        <v>154</v>
-      </c>
       <c r="C10" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="28" t="s">
         <v>135</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>136</v>
       </c>
       <c r="E10" s="28">
         <v>1</v>
@@ -5557,16 +5823,16 @@
     </row>
     <row r="11" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="28" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" s="28" t="s">
+      <c r="D11" s="28" t="s">
         <v>156</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>157</v>
       </c>
       <c r="E11" s="28">
         <v>2</v>
@@ -5574,13 +5840,13 @@
     </row>
     <row r="12" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="28" t="s">
-        <v>159</v>
-      </c>
       <c r="C12" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12" s="28">
         <v>4</v>
@@ -5588,16 +5854,16 @@
     </row>
     <row r="13" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="C13" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>161</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>162</v>
       </c>
       <c r="E13" s="28">
         <v>2</v>
@@ -5605,16 +5871,16 @@
     </row>
     <row r="14" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B14" s="28">
         <v>600</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E14" s="28">
         <v>4</v>
@@ -5622,16 +5888,16 @@
     </row>
     <row r="15" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B15" s="28">
         <v>120</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E15" s="28">
         <v>2</v>
@@ -5639,16 +5905,16 @@
     </row>
     <row r="16" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>165</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="D16" s="28" t="s">
         <v>167</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>168</v>
       </c>
       <c r="E16" s="28">
         <v>1</v>
@@ -5680,36 +5946,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>127</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" s="29" t="s">
         <v>169</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="C2" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>170</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>171</v>
       </c>
       <c r="E2" s="29">
         <v>8</v>
@@ -5718,16 +5984,16 @@
     </row>
     <row r="3" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="C3" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D3" s="29" t="s">
         <v>173</v>
-      </c>
-      <c r="C3" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="E3" s="29">
         <v>2</v>
@@ -5736,16 +6002,16 @@
     </row>
     <row r="4" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="29" t="s">
+        <v>174</v>
+      </c>
+      <c r="B4" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>176</v>
-      </c>
       <c r="C4" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E4" s="29">
         <v>1</v>
@@ -5754,16 +6020,16 @@
     </row>
     <row r="5" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>178</v>
-      </c>
       <c r="C5" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E5" s="29">
         <v>2</v>
@@ -5772,16 +6038,16 @@
     </row>
     <row r="6" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="C6" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="29" t="s">
         <v>180</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>181</v>
       </c>
       <c r="E6" s="29">
         <v>1</v>
@@ -5790,16 +6056,16 @@
     </row>
     <row r="7" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>183</v>
-      </c>
       <c r="C7" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" s="29">
         <v>1</v>
@@ -5808,16 +6074,16 @@
     </row>
     <row r="8" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B8" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="29" t="s">
-        <v>185</v>
-      </c>
       <c r="C8" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E8" s="29">
         <v>2</v>
@@ -5826,16 +6092,16 @@
     </row>
     <row r="9" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="B9" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="C9" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="29" t="s">
         <v>187</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>188</v>
       </c>
       <c r="E9" s="29">
         <v>4</v>
@@ -5844,16 +6110,16 @@
     </row>
     <row r="10" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="29" t="s">
         <v>189</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>190</v>
       </c>
       <c r="E10" s="29">
         <v>1</v>
@@ -5862,16 +6128,16 @@
     </row>
     <row r="11" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="29" t="s">
         <v>191</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>192</v>
       </c>
       <c r="E11" s="29">
         <v>1</v>
@@ -5880,16 +6146,16 @@
     </row>
     <row r="12" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B12" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="29" t="s">
         <v>193</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="29" t="s">
-        <v>194</v>
       </c>
       <c r="E12" s="29">
         <v>1</v>
@@ -5898,16 +6164,16 @@
     </row>
     <row r="13" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>195</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>196</v>
-      </c>
       <c r="C13" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E13" s="29">
         <v>1</v>
@@ -5916,16 +6182,16 @@
     </row>
     <row r="14" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B14" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="B14" s="29" t="s">
-        <v>198</v>
-      </c>
       <c r="C14" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D14" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E14" s="29">
         <v>1</v>
@@ -5934,16 +6200,16 @@
     </row>
     <row r="15" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D15" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="29">
         <v>1</v>
@@ -5952,16 +6218,16 @@
     </row>
     <row r="16" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" s="29">
         <v>1</v>
@@ -5970,16 +6236,16 @@
     </row>
     <row r="17" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D17" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E17" s="29">
         <v>1</v>
@@ -5988,16 +6254,16 @@
     </row>
     <row r="18" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="B18" s="29" t="s">
         <v>202</v>
       </c>
-      <c r="B18" s="29" t="s">
-        <v>203</v>
-      </c>
       <c r="C18" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D18" s="29" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E18" s="29">
         <v>1</v>
@@ -6006,16 +6272,16 @@
     </row>
     <row r="19" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="B19" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="C19" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="31" t="s">
         <v>205</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>206</v>
       </c>
       <c r="E19" s="31">
         <v>1</v>
@@ -6024,16 +6290,16 @@
     </row>
     <row r="20" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B20" s="29" t="s">
         <v>207</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="C20" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="29" t="s">
         <v>208</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D20" s="29" t="s">
-        <v>209</v>
       </c>
       <c r="E20" s="29">
         <v>1</v>
@@ -6042,14 +6308,14 @@
     </row>
     <row r="21" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" s="29" t="s">
         <v>210</v>
-      </c>
-      <c r="B21" s="29" t="s">
-        <v>211</v>
       </c>
       <c r="C21" s="29"/>
       <c r="D21" s="29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E21" s="29">
         <v>4</v>
@@ -6058,16 +6324,16 @@
     </row>
     <row r="22" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="B22" s="29" t="s">
-        <v>214</v>
-      </c>
       <c r="C22" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E22" s="29">
         <v>1</v>
@@ -6076,16 +6342,16 @@
     </row>
     <row r="23" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B23" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="29" t="s">
         <v>161</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="D23" s="29" t="s">
-        <v>162</v>
       </c>
       <c r="E23" s="29">
         <v>9</v>
@@ -6094,16 +6360,16 @@
     </row>
     <row r="24" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="29" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B24" s="29">
         <v>600</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E24" s="29">
         <v>4</v>
@@ -6112,16 +6378,16 @@
     </row>
     <row r="25" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="29" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B25" s="29">
         <v>120</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E25" s="29">
         <v>2</v>
@@ -6130,16 +6396,16 @@
     </row>
     <row r="26" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E26" s="29">
         <v>1</v>
@@ -6148,16 +6414,16 @@
     </row>
     <row r="27" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B27" s="29">
         <v>330</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E27" s="29">
         <v>3</v>
@@ -6166,16 +6432,16 @@
     </row>
     <row r="28" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="B28" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="C28" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="D28" s="29" t="s">
         <v>167</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>168</v>
       </c>
       <c r="E28" s="29">
         <v>1</v>
@@ -6184,7 +6450,7 @@
     </row>
     <row r="29" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B29" s="29" t="s">
         <v>51</v>
@@ -6193,7 +6459,7 @@
         <v>51</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E29" s="29">
         <v>1</v>
@@ -6202,16 +6468,16 @@
     </row>
     <row r="30" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B30" s="29" t="s">
         <v>222</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="C30" s="29" t="s">
         <v>223</v>
       </c>
-      <c r="C30" s="29" t="s">
-        <v>224</v>
-      </c>
       <c r="D30" s="29" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E30" s="29">
         <v>1</v>
@@ -6220,16 +6486,16 @@
     </row>
     <row r="31" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B31" s="29" t="s">
         <v>50</v>
       </c>
       <c r="C31" s="29" t="s">
+        <v>225</v>
+      </c>
+      <c r="D31" s="29" t="s">
         <v>226</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>227</v>
       </c>
       <c r="E31" s="29">
         <v>1</v>
@@ -6238,16 +6504,16 @@
     </row>
     <row r="32" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" s="29" t="s">
         <v>228</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="C32" s="29" t="s">
         <v>229</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="D32" s="29" t="s">
         <v>230</v>
-      </c>
-      <c r="D32" s="29" t="s">
-        <v>231</v>
       </c>
       <c r="E32" s="29">
         <v>1</v>

</xml_diff>